<commit_message>
EXCEL ABS DESPUES STN
</commit_message>
<xml_diff>
--- a/datos_extraidos.xlsx
+++ b/datos_extraidos.xlsx
@@ -451,27 +451,27 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>ABS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Punto</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Código</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>STK</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Stn</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre Punto</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Código</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>STK</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ABS</t>
         </is>
       </c>
     </row>
@@ -493,27 +493,27 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>338.60</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S233</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TISS INFILTRACIC</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S233 TISS INFILTRACIC</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>K3+38.60</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S233</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>TISS INFILTRACIC</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S233 TISS INFILTRACIC</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>338.60</t>
         </is>
       </c>
     </row>
@@ -535,27 +535,27 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>332.88</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S232</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>POZO 1</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S232 POZO 1</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>K3+32.88</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S232</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>POZO 1</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S232 POZO 1</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>332.88</t>
         </is>
       </c>
     </row>
@@ -577,27 +577,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>452.73</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S234</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>POZO 2</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S234 POZO 2</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>K4+52.73</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S234</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>POZO 2</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S234 POZO 2</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>452.73</t>
         </is>
       </c>
     </row>
@@ -619,27 +619,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>131.37</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S241</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>VDC 2</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>STK_03-08-25-S241 VDC 2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>K1+31.37</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S241</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>VDC 2</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>STK_03-08-25-S241 VDC 2</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>131.37</t>
         </is>
       </c>
     </row>
@@ -661,27 +661,27 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>143.28</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>STK_03-08-2025-251@</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>VDC 1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>STK_03-08-2025-251@ VDC 1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
           <t>K1+43.28</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>STK_03-08-2025-251@</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>VDC 1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>STK_03-08-2025-251@ VDC 1</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>143.28</t>
         </is>
       </c>
     </row>

</xml_diff>